<commit_message>
Included code and explanation for call by reference
</commit_message>
<xml_diff>
--- a/pointers/explanation.xlsx
+++ b/pointers/explanation.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="basic_pointer" sheetId="1" r:id="rId1"/>
     <sheet name="pointer_arthemetic" sheetId="2" r:id="rId2"/>
     <sheet name="pointer_typescast" sheetId="3" r:id="rId3"/>
+    <sheet name="call_by_value" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>RAM</t>
   </si>
@@ -189,12 +190,51 @@
   <si>
     <t>Note:- Each block is 1 byte</t>
   </si>
+  <si>
+    <t>#include&lt;stdio.h&gt;
+#include&lt;conio.h&gt;
+void inc(int);
+void main()
+{
+ int a=10;
+ printf("In main function--&gt;address of a=%x, a=%d\n", &amp;a, a);
+ inc(a);
+ printf("In main function--&gt;address of a=%x, a=%d\n", &amp;a, a);
+}
+void inc(int a)
+{
+ printf("In Inc function--&gt;address of a=%x, a=%d\n", &amp;a, a);
+ a=a+5;
+ printf("In Inc function--&gt;address of a=%x, a=%d\n", &amp;a, a);
+}</t>
+  </si>
+  <si>
+    <t>$ ./call_by_value.exe</t>
+  </si>
+  <si>
+    <t>In main function--&gt;address of a=61ff1c, a=10</t>
+  </si>
+  <si>
+    <t>In Inc function--&gt;address of a=61ff00, a=10</t>
+  </si>
+  <si>
+    <t>In Inc function--&gt;address of a=61ff00, a=15</t>
+  </si>
+  <si>
+    <t>0x61ff00</t>
+  </si>
+  <si>
+    <t>main function</t>
+  </si>
+  <si>
+    <t>inc function</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +261,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -323,7 +371,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -352,12 +400,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -369,6 +411,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -377,6 +425,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -675,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -686,102 +740,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
       <c r="L2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
       <c r="K8" s="9" t="s">
         <v>13</v>
       </c>
@@ -793,15 +847,15 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
       <c r="K9" s="9" t="s">
         <v>1</v>
       </c>
@@ -813,75 +867,75 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:13">
@@ -1200,108 +1254,108 @@
   <dimension ref="A2:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:P23"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
       <c r="L3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
       <c r="K9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1313,15 +1367,15 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
       <c r="K10" s="9" t="s">
         <v>1</v>
       </c>
@@ -1333,15 +1387,15 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
       <c r="L11" s="7">
         <v>6422284</v>
       </c>
@@ -1353,63 +1407,63 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12">
@@ -1455,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1465,357 +1519,357 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="L3" s="13" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="L3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="13" t="s">
         <v>33</v>
       </c>
       <c r="L6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="15"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13"/>
       <c r="L7" s="20"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="15"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
       <c r="L8" s="20"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13" t="s">
         <v>13</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
       <c r="L11" s="20"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="20"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="15"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="21"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="15" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="14" t="s">
+      <c r="M14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="17" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M15" s="14" t="s">
+      <c r="M15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="17" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
     </row>
     <row r="17" spans="1:16" ht="15" thickBot="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="18" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="7" t="s">
@@ -1824,13 +1878,13 @@
       <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="7" t="s">
@@ -1839,37 +1893,37 @@
       <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="14"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="7" t="s">
@@ -1890,4 +1944,365 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="L2" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="19">
+        <v>10</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="22"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="22"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="22"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="19">
+        <v>15</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="22"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="22"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="22"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="12"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="12"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="12"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="12"/>
+      <c r="J19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:I17"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="L9:L12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="N5:N8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated call value program with some prints
</commit_message>
<xml_diff>
--- a/pointers/explanation.xlsx
+++ b/pointers/explanation.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="basic_pointer" sheetId="1" r:id="rId1"/>
     <sheet name="pointer_arthemetic" sheetId="2" r:id="rId2"/>
     <sheet name="pointer_typescast" sheetId="3" r:id="rId3"/>
     <sheet name="call_by_value" sheetId="4" r:id="rId4"/>
+    <sheet name="call_by_reference" sheetId="5" r:id="rId5"/>
+    <sheet name="pointer&amp;arrays" sheetId="6" r:id="rId6"/>
+    <sheet name="array_as_fun_argument" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
   <si>
     <t>RAM</t>
   </si>
@@ -218,9 +221,6 @@
     <t>In Inc function--&gt;address of a=61ff00, a=10</t>
   </si>
   <si>
-    <t>In Inc function--&gt;address of a=61ff00, a=15</t>
-  </si>
-  <si>
     <t>0x61ff00</t>
   </si>
   <si>
@@ -228,6 +228,232 @@
   </si>
   <si>
     <t>inc function</t>
+  </si>
+  <si>
+    <t>In Inc function after a=a+5 --&gt;address of a=61ff00, a=15</t>
+  </si>
+  <si>
+    <t>In main function after executing inc function --&gt;address of a=61ff1c, a=10</t>
+  </si>
+  <si>
+    <t>$ ./call_by_reference.exe</t>
+  </si>
+  <si>
+    <t>In Inc function--&gt;address of a=61ff00, a=61ff1c *a=10</t>
+  </si>
+  <si>
+    <t>In Inc function after *a=*a+5 --&gt;address of a=61ff00, a=61ff1c *a=15</t>
+  </si>
+  <si>
+    <t>In main function after executing inc function --&gt;address of a=61ff1c, a=15</t>
+  </si>
+  <si>
+    <t>#include&lt;stdio.h&gt;
+#include&lt;conio.h&gt;
+void inc(int*);
+void main()
+{
+ int a=10;
+ printf("In main function--&gt;address of a=%x, a=%d\n", &amp;a, a);
+ inc(&amp;a);
+ printf("In main function after executing inc function --&gt;address of a=%x, a=%d\n", &amp;a, a);
+}
+void inc(int *a)
+{
+ printf("In Inc function--&gt;address of a=%x, a=%x *a=%d\n", &amp;a, a, *a);
+ *a=*a+5;
+ printf("In Inc function after *a=*a+5 --&gt;address of a=%x, a=%x *a=%d\n", &amp;a, a, *a );
+}</t>
+  </si>
+  <si>
+    <t>(10) - value replaced</t>
+  </si>
+  <si>
+    <t>(10)  15</t>
+  </si>
+  <si>
+    <t>( ) indicates value replaced</t>
+  </si>
+  <si>
+    <t>hrupa@Roopak MINGW32 /d/c_codes/repo/c-language-programs/pointers (master)</t>
+  </si>
+  <si>
+    <t>$ ./pointer_and_arrays.exe</t>
+  </si>
+  <si>
+    <t>&amp;a[i]=61ff08, a[i]=1    a+i=61ff08, *(a+i)=1</t>
+  </si>
+  <si>
+    <t>&amp;a[i]=61ff0c, a[i]=2    a+i=61ff0c, *(a+i)=2</t>
+  </si>
+  <si>
+    <t>&amp;a[i]=61ff10, a[i]=3    a+i=61ff10, *(a+i)=3</t>
+  </si>
+  <si>
+    <t>&amp;a[i]=61ff14, a[i]=4    a+i=61ff14, *(a+i)=4</t>
+  </si>
+  <si>
+    <t>&amp;a[i]=61ff18, a[i]=5    a+i=61ff18, *(a+i)=5</t>
+  </si>
+  <si>
+    <t>Note: If a array is defined then its variable is treated pointer variable</t>
+  </si>
+  <si>
+    <t>Note:- Each block is 4 byte</t>
+  </si>
+  <si>
+    <t>0x61ff08</t>
+  </si>
+  <si>
+    <t>0x61ff0c</t>
+  </si>
+  <si>
+    <t>0x61ff10</t>
+  </si>
+  <si>
+    <t>address of a=61ff08 value of a=61ff08</t>
+  </si>
+  <si>
+    <t>#include&lt;stdio.h&gt;
+#include&lt;conio.h&gt;
+void main()
+{
+ int a[]={1,2,3,4,5};
+printf("address of a=%x value of a=%x\n", &amp;a, a);
+ for(int i=0;i&lt;5;i++)
+  {
+      printf("&amp;a[i]=%x, a[i]=%d\t",&amp;a[i], a[i]);
+      printf("a+i=%x, *(a+i)=%d\n",a+i, *(a+i));
+  }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We cant perform post , pre increament or decreament on array variable </t>
+  </si>
+  <si>
+    <t>$ ./array_as_function_argument.exe</t>
+  </si>
+  <si>
+    <t>Address of a=61ff08 value of a=61ff08</t>
+  </si>
+  <si>
+    <t>[In main function] sizeof(a)=20, sizeof(a[0]) = 4</t>
+  </si>
+  <si>
+    <t>[In SumOfElements function] sizeof(a)=4, sizeof(a[0]) = 4</t>
+  </si>
+  <si>
+    <t>Sum of Elements = 15</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>(1)(3)(6)(10) 15</t>
+  </si>
+  <si>
+    <t>Note:-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Each block is 4 byte</t>
+  </si>
+  <si>
+    <t>[In main function] size of array=5</t>
+  </si>
+  <si>
+    <t>[In SumOfElements function] size of array=5</t>
+  </si>
+  <si>
+    <t>output for program 1</t>
+  </si>
+  <si>
+    <t>output for program 2</t>
+  </si>
+  <si>
+    <t>SumOfElements</t>
+  </si>
+  <si>
+    <t>Program 1</t>
+  </si>
+  <si>
+    <t>Program 2</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>size_of_array</t>
+  </si>
+  <si>
+    <t>(garbage) 15</t>
+  </si>
+  <si>
+    <t>[In SumOfElements function] size of array=1</t>
+  </si>
+  <si>
+    <t>Sum of Elements = 1</t>
+  </si>
+  <si>
+    <t>#include&lt;stdio.h&gt;
+#include&lt;conio.h&gt;
+#define PROGRAM1 1
+#define PROGRAM2 0
+#if PROGRAM1
+int SumOfElements(int *);
+SumOfElements(int a[]) // int a[] or int *a
+{
+ int sum=0,size_of_array=0;
+ printf("[In SumOfElements function] sizeof(a)=%d, sizeof(a[0]) = %x\n", sizeof(a), sizeof(a[0])); 
+ // As we dont pass entire array to this function , we just pass address of array to a , so sizeof a will be 4 bytes , its like pointer variable
+ size_of_array = sizeof(a)/sizeof(a[0]);
+ printf("[In SumOfElements function] size of array=%d\n", size_of_array); 
+ for(int i=0; i&lt;size_of_array; i++)
+ {
+  sum+=*(a+i);
+ }
+ return sum;
+}
+void main()
+{
+ int a[]={1,2,3,4,5}, total;
+ printf("Address of a=%x value of a=%x\n", &amp;a, a);
+ printf("[In main function] sizeof(a)=%d, sizeof(a[0]) = %x\n", sizeof(a), sizeof(a[0]));
+ printf("[In main function] size of array=%d\n", sizeof(a)/sizeof(a[0])); 
+ total = SumOfElements(a);
+ printf("Sum of Elements = %d\n", total);
+}
+#endif
+#if PROGRAM2
+int SumOfElements(int *, int);
+SumOfElements(int a[], int size) // int a[] or int *a
+{
+ int sum=0, size_of_array;
+ printf("[In SumOfElements function] sizeof(a)=%d, sizeof(a[0]) = %x\n", sizeof(a), sizeof(a[0])); 
+ // As we dont pass entire array to this function , we just pass address of array to a , so sizeof a will be 4 bytes , its like pointer variable
+ size_of_array = size/sizeof(a);
+ printf("[In SumOfElements function] size of array=%d\n", size_of_array); 
+ for(int i=0; i&lt;size_of_array; i++)
+ {
+  sum+=*(a+i);
+ }
+ return sum;
+}
+void main()
+{
+ int a[]={1,2,3,4,5}, total;
+ printf("Address of a=%x value of a=%x\n", &amp;a, a);
+ printf("[In main function] sizeof(a)=%d, sizeof(a[0]) = %x\n", sizeof(a), sizeof(a[0]));
+ printf("[In main function] size of array=%d\n", sizeof(a)/sizeof(a[0])); 
+ total = SumOfElements(a, sizeof(a));
+ printf("Sum of Elements = %d\n", total);
+}
+#endif</t>
   </si>
 </sst>
 </file>
@@ -271,12 +497,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -371,7 +627,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -411,6 +667,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -429,8 +726,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -740,102 +1040,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
       <c r="L2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="K8" s="9" t="s">
         <v>13</v>
       </c>
@@ -847,15 +1147,15 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
       <c r="K9" s="9" t="s">
         <v>1</v>
       </c>
@@ -867,75 +1167,75 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:13">
@@ -1260,102 +1560,102 @@
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="2" spans="1:14">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="L3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
       <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
       <c r="K9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1367,15 +1667,15 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
       <c r="K10" s="9" t="s">
         <v>1</v>
       </c>
@@ -1387,15 +1687,15 @@
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
       <c r="L11" s="7">
         <v>6422284</v>
       </c>
@@ -1407,63 +1707,63 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="1:12">
@@ -1519,42 +1819,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="14.4" customHeight="1">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
       <c r="L3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
@@ -1564,15 +1864,15 @@
       <c r="P4" s="12"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
@@ -1582,20 +1882,20 @@
       <c r="P5" s="12"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="12"/>
       <c r="K6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="36" t="s">
         <v>15</v>
       </c>
       <c r="M6" s="12" t="s">
@@ -1606,74 +1906,74 @@
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="12"/>
       <c r="K7" s="13"/>
-      <c r="L7" s="20"/>
+      <c r="L7" s="37"/>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="12"/>
       <c r="K8" s="13"/>
-      <c r="L8" s="20"/>
+      <c r="L8" s="37"/>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
       <c r="J9" s="12"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="21"/>
+      <c r="L9" s="38"/>
       <c r="M9" s="14"/>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
       <c r="J10" s="12"/>
       <c r="K10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="36" t="s">
         <v>15</v>
       </c>
       <c r="M10" s="14" t="s">
@@ -1684,69 +1984,69 @@
       <c r="P10" s="12"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="12"/>
       <c r="K11" s="13"/>
-      <c r="L11" s="20"/>
+      <c r="L11" s="37"/>
       <c r="M11" s="14"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="12"/>
       <c r="K12" s="13"/>
-      <c r="L12" s="20"/>
+      <c r="L12" s="37"/>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
       <c r="J13" s="12"/>
       <c r="K13" s="13"/>
-      <c r="L13" s="21"/>
+      <c r="L13" s="38"/>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="12"/>
       <c r="K14" s="13" t="s">
         <v>1</v>
@@ -1762,15 +2062,15 @@
       <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="15" t="s">
@@ -1784,15 +2084,15 @@
       <c r="P15" s="12"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="15" t="s">
@@ -1806,15 +2106,15 @@
       <c r="P16" s="12"/>
     </row>
     <row r="17" spans="1:16" ht="15" thickBot="1">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="16" t="s">
@@ -1828,15 +2128,15 @@
       <c r="P17" s="12"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -1948,310 +2248,217 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="113.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:9" ht="14.4" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="L2" s="11" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="34"/>
+      <c r="B2" s="3"/>
+      <c r="E2" s="11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13" t="s">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="34"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="34"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="34"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="19">
+      <c r="E5" s="36">
         <v>10</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="G5" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="34"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="39"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="34"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="39"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="34"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="39"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="34"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="36">
+        <v>15</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="39" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="22"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="22"/>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="22"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="19">
-        <v>15</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="22"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="22"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="12"/>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="12"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="12"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="12"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="34"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="39"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="34"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="39"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="34"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="39"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="34"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="12"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="34"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="12"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="34"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="12"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1">
+      <c r="A16" s="34"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="12"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" t="s">
+      <c r="A18" s="34"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="12"/>
-      <c r="J19" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="7" t="s">
         <v>47</v>
       </c>
       <c r="J20" s="12"/>
@@ -2260,7 +2467,7 @@
       <c r="M20" s="12"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="7" t="s">
         <v>48</v>
       </c>
       <c r="J21" s="12"/>
@@ -2269,7 +2476,7 @@
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="7" t="s">
         <v>49</v>
       </c>
       <c r="J22" s="12"/>
@@ -2278,8 +2485,8 @@
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="12" t="s">
-        <v>50</v>
+      <c r="A23" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
@@ -2287,8 +2494,8 @@
       <c r="M23" s="12"/>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="12" t="s">
-        <v>48</v>
+      <c r="A24" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2296,13 +2503,1013 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:I17"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="L9:L12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="N5:N8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="A1:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="109.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="34"/>
+      <c r="B2" s="3"/>
+      <c r="E2" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="34"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="34"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="34"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="34"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="39"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="34"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="39"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="34"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="39"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="34"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="34"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="39"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="34"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="39"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="34"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="34"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="34"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="34"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1">
+      <c r="A16" s="34"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="34"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="34"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A18"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="G5:G8"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="G9:G12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="91.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="34"/>
+      <c r="B2" s="3"/>
+      <c r="E2" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="34"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="34"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="34"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="20">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="34"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="20">
+        <v>2</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="34"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="20">
+        <v>3</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="34"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="20">
+        <v>4</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="34"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="20">
+        <v>5</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="34"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="34"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="34"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="34"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="34"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="34"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="34"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="34"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="34"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="116.77734375" customWidth="1"/>
+    <col min="2" max="2" width="68.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="34"/>
+      <c r="B2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="34"/>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="34"/>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="34"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21">
+        <v>1</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="34"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="21">
+        <v>2</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="40"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="34"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="21">
+        <v>3</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="40"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="34"/>
+      <c r="B8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="21">
+        <v>4</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="40"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="34"/>
+      <c r="B9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="21">
+        <v>5</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="40"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="34"/>
+      <c r="B10" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="40"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="34"/>
+      <c r="B11" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="40"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="34"/>
+      <c r="B12" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="34"/>
+      <c r="B13" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="40"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="34"/>
+      <c r="B14" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="40"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="34"/>
+      <c r="B15" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="34"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="34"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="34"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="34"/>
+      <c r="B19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="34"/>
+      <c r="B20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="34"/>
+      <c r="B21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="34"/>
+      <c r="B22" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="34"/>
+      <c r="B23" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="34"/>
+      <c r="B24" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="21">
+        <v>1</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="34"/>
+      <c r="B25" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="21">
+        <v>2</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" s="40"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="34"/>
+      <c r="B26" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="21">
+        <v>3</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="40"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="34"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="21">
+        <v>4</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="40"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="34"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="21">
+        <v>5</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="40"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="34"/>
+      <c r="D29" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="31"/>
+      <c r="G29" s="40"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="34"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="40"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="34"/>
+      <c r="D31" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="23"/>
+      <c r="G31" s="40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="34"/>
+      <c r="D32" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="24">
+        <v>20</v>
+      </c>
+      <c r="F32" s="23"/>
+      <c r="G32" s="40"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="34"/>
+      <c r="D33" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="23"/>
+      <c r="G33" s="40"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="34"/>
+      <c r="D34" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="24">
+        <v>5</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" s="40"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="34"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="34"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="34"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="34"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="34"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="34"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="34"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="34"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="34"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="34"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="34"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="34"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="34"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="34"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="34"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="34"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="34"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="34"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="34"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="34"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="34"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="34"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="34"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="34"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="34"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:A60"/>
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="G5:G11"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G24:G30"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D20:G20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Included some basic concepts of strings
</commit_message>
<xml_diff>
--- a/pointers/explanation.xlsx
+++ b/pointers/explanation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="basic_pointer" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="call_by_reference" sheetId="5" r:id="rId5"/>
     <sheet name="pointer&amp;arrays" sheetId="6" r:id="rId6"/>
     <sheet name="array_as_fun_argument" sheetId="7" r:id="rId7"/>
+    <sheet name="strings&amp;pointers" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="142">
   <si>
     <t>RAM</t>
   </si>
@@ -455,6 +456,126 @@
 }
 #endif</t>
   </si>
+  <si>
+    <t>string size is Size of array &gt;= no:of charcters in string +1</t>
+  </si>
+  <si>
+    <t>A string in c has to be null terminated as below</t>
+  </si>
+  <si>
+    <t>char ch[] = {"a","b","c","d","e","f","\0"}</t>
+  </si>
+  <si>
+    <t>we can print the above string using printf("%s"); if we dont give "\0" then it will print garbage value</t>
+  </si>
+  <si>
+    <t>int main()</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>char ch[3];</t>
+  </si>
+  <si>
+    <t>ch[0]='a';</t>
+  </si>
+  <si>
+    <t>printf("%s", ch);</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>abc^&amp;*#@</t>
+  </si>
+  <si>
+    <t>Note: After abc we see garbage value</t>
+  </si>
+  <si>
+    <t>ch[1]='b';</t>
+  </si>
+  <si>
+    <t>ch[2]='c';</t>
+  </si>
+  <si>
+    <t>ch[3]='\0';</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>char ch[4]; // char ch[20]; -&gt; this is allowed</t>
+  </si>
+  <si>
+    <t>printf("String length - %d", strlen(ch));</t>
+  </si>
+  <si>
+    <t>printf("%s\n", ch);</t>
+  </si>
+  <si>
+    <t>String length - 3</t>
+  </si>
+  <si>
+    <t>program 1</t>
+  </si>
+  <si>
+    <t>program 2</t>
+  </si>
+  <si>
+    <t>program 3</t>
+  </si>
+  <si>
+    <t>roopak</t>
+  </si>
+  <si>
+    <t>String length - 6</t>
+  </si>
+  <si>
+    <t>char ch[20];</t>
+  </si>
+  <si>
+    <t>ch = "roopak"; // This is invalid, it should be done as program 3</t>
+  </si>
+  <si>
+    <t>program 4</t>
+  </si>
+  <si>
+    <t>char ch[]="roopak"; // As this is a string it will add "\0" at the end of the string</t>
+  </si>
+  <si>
+    <t>#include&lt;stdio.h&gt;</t>
+  </si>
+  <si>
+    <t>#include&lt;conio.h&gt;</t>
+  </si>
+  <si>
+    <t>#include&lt;string.h&gt;</t>
+  </si>
+  <si>
+    <t>void main()</t>
+  </si>
+  <si>
+    <t>char ch[] = "cooding";</t>
+  </si>
+  <si>
+    <t>printf("sizeof string = %d , length of the string = %d\n", sizeof(ch), strlen(ch));</t>
+  </si>
+  <si>
+    <t>$ ./pointers_and_strings</t>
+  </si>
+  <si>
+    <t>cooding</t>
+  </si>
+  <si>
+    <t>sizeof string = 8 , length of the string = 7</t>
+  </si>
+  <si>
+    <t>sizeof of the string is 8 becasue no:of charecters in the string is 7 + 1 null charecter</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
 </sst>
 </file>
 
@@ -497,7 +618,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -531,6 +652,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,7 +754,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -731,6 +858,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3012,7 +3143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -3512,4 +3643,314 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:C50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="2" width="59.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Included one more program for string with address and values
</commit_message>
<xml_diff>
--- a/pointers/explanation.xlsx
+++ b/pointers/explanation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="169">
   <si>
     <t>RAM</t>
   </si>
@@ -575,6 +575,87 @@
   </si>
   <si>
     <t>Note:</t>
+  </si>
+  <si>
+    <t>printf("&amp;ch = %x, ch=%d\n", &amp;ch, ch);</t>
+  </si>
+  <si>
+    <t>for(int i=0; i &lt;= sizeof(ch)-1; i++)</t>
+  </si>
+  <si>
+    <t>printf("&amp;(ch+i)=%x, *(ch+i)=%c\n", (ch+i), *(ch+i));</t>
+  </si>
+  <si>
+    <t>$ ./pointers_and_strings_1</t>
+  </si>
+  <si>
+    <t>&amp;ch = 61ff14, ch=6422292</t>
+  </si>
+  <si>
+    <t>&amp;(ch+i)=61ff14, *(ch+i)=c</t>
+  </si>
+  <si>
+    <t>&amp;(ch+i)=61ff15, *(ch+i)=o</t>
+  </si>
+  <si>
+    <t>&amp;(ch+i)=61ff16, *(ch+i)=o</t>
+  </si>
+  <si>
+    <t>&amp;(ch+i)=61ff17, *(ch+i)=d</t>
+  </si>
+  <si>
+    <t>&amp;(ch+i)=61ff18, *(ch+i)=i</t>
+  </si>
+  <si>
+    <t>&amp;(ch+i)=61ff19, *(ch+i)=n</t>
+  </si>
+  <si>
+    <t>&amp;(ch+i)=61ff1a, *(ch+i)=g</t>
+  </si>
+  <si>
+    <t>&amp;(ch+i)=61ff1b, *(ch+i)=</t>
+  </si>
+  <si>
+    <t>61ff14</t>
+  </si>
+  <si>
+    <t>61ff15</t>
+  </si>
+  <si>
+    <t>61ff16</t>
+  </si>
+  <si>
+    <t>61ff17</t>
+  </si>
+  <si>
+    <t>61ff18</t>
+  </si>
+  <si>
+    <t>61ff19</t>
+  </si>
+  <si>
+    <t>61ff1a</t>
+  </si>
+  <si>
+    <t>61ff1b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -754,7 +835,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -862,6 +943,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3144,7 +3228,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3647,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C50"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3658,6 +3742,11 @@
     <col min="1" max="2" width="59.6640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>102</v>
@@ -3748,7 +3837,7 @@
       <c r="A12" t="s">
         <v>115</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3756,7 +3845,7 @@
       <c r="A13" t="s">
         <v>110</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3764,7 +3853,7 @@
       <c r="A14" t="s">
         <v>111</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3776,7 +3865,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>112</v>
       </c>
@@ -3784,157 +3873,310 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="B21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="B22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="B25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="B26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="B27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="B29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="F31" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I33" s="44" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I34" s="44"/>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I35" s="44"/>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I36" s="44"/>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="I37" s="44"/>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="I38" s="44"/>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="I39" s="44"/>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I40" s="44"/>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:9">
       <c r="A47" s="42" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>120</v>
       </c>
@@ -3950,6 +4192,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I33:I40"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>